<commit_message>
fixed duplicate5b-7 to 5a-7
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_fullrun_hbrown_01.13.20.xlsx
+++ b/fastqFiles/fastq_fullrun_hbrown_01.13.20.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A904CFE1-8FC4-3C48-8E1F-1A43FE2E682D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655629BD-2167-DD4D-87CE-4B27C09EFFDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32440" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32440" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="69">
   <si>
     <t>libraryDate</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Brent_large/Brent_5b-26_GTAC_26_SIC_Index2_07_TCAACTG_GAGTTGGT_S53_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_small/Brent_5a-7_GTAC_7_SIC_Index2_08_AGACTGA_AAGCACGT_S8_R1_001.fastq.gz:5700146</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
   <dimension ref="A1:Y53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +960,7 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
@@ -969,7 +972,7 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="G8" t="s">
@@ -978,14 +981,14 @@
       <c r="H8">
         <v>0.25600000000000001</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8">
         <v>6.5612298143469197</v>
       </c>
       <c r="J8">
         <v>5700146</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>22</v>
+      <c r="K8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>